<commit_message>
TP3 Q1 & Q2 done
</commit_message>
<xml_diff>
--- a/TP3/TP3_3430.xlsx
+++ b/TP3/TP3_3430.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\Bureau\log3430\TP3\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workspace\POLY\H19\LOG3430\Labos\TP3\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A814302-7896-4666-B0E4-B934DE35E630}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12330"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12330" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -98,7 +99,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -439,11 +440,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -588,56 +589,66 @@
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="A6" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B6" t="s">
-        <v>19</v>
-      </c>
-      <c r="C6" t="s">
-        <v>19</v>
-      </c>
-      <c r="D6" t="s">
-        <v>19</v>
-      </c>
-      <c r="H6" t="s">
+      <c r="B6" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="I6" t="s">
+      <c r="I6" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="J6" t="s">
+      <c r="J6" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="L6" t="s">
+      <c r="K6" s="2"/>
+      <c r="L6" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="M6" t="s">
+      <c r="M6" s="2" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="A7" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B7" t="s">
-        <v>19</v>
-      </c>
-      <c r="C7" t="s">
-        <v>19</v>
-      </c>
-      <c r="D7" t="s">
-        <v>19</v>
-      </c>
-      <c r="H7" t="s">
+      <c r="B7" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="K7" t="s">
+      <c r="I7" s="2"/>
+      <c r="J7" s="2"/>
+      <c r="K7" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="L7" t="s">
+      <c r="L7" s="2" t="s">
         <v>22</v>
       </c>
+      <c r="M7" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>